<commit_message>
list time change and put data into arrays
</commit_message>
<xml_diff>
--- a/flight list.xlsx
+++ b/flight list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alonn\OneDrive\Desktop\380\380Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2030CD08-C404-4527-BF48-DAD7EDB23AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97578943-7268-486C-9F72-9AB72623AB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{3E2F1562-5331-48AA-A055-332B17C62621}"/>
+    <workbookView xWindow="4110" yWindow="30" windowWidth="21600" windowHeight="11295" xr2:uid="{3E2F1562-5331-48AA-A055-332B17C62621}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -572,25 +572,25 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,22 +905,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517DFADA-824D-4267-906F-77924C906201}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="3"/>
-    <col min="5" max="8" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,1563 +945,1564 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:9" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>45214</v>
       </c>
       <c r="F2" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>45214</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="5">
         <v>0.64583333333333337</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>45215</v>
       </c>
       <c r="F3" s="6">
         <v>0.4375</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>45215</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <v>0.59375</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:9" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>45217</v>
       </c>
       <c r="F4" s="6">
         <v>0.82291666666666663</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>45218</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <v>0.6875</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:9" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>45219</v>
       </c>
       <c r="F5" s="6">
         <v>0.95833333333333337</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>45220</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <v>0.65625</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:9" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>45216</v>
       </c>
       <c r="F6" s="6">
         <v>0.38541666666666669</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>45216</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <v>0.44791666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:9" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4">
         <v>45218</v>
       </c>
       <c r="F7" s="6">
         <v>0.5625</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>45218</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <v>0.69791666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:9" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>45221</v>
       </c>
       <c r="F8" s="6">
         <v>0.375</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>45222</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <v>0.6875</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:9" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4">
         <v>45223</v>
       </c>
       <c r="F9" s="6">
         <v>0.86458333333333337</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>45223</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>0.63541666666666663</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:9" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>45225</v>
       </c>
       <c r="F10" s="6">
         <v>0.97916666666666663</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>45226</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <v>0.17708333333333334</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:9" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="5">
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4">
         <v>45227</v>
       </c>
       <c r="F11" s="6">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>45227</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <v>0.65625</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:9" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>45229</v>
       </c>
       <c r="F12" s="6">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>45229</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <v>0.57291666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:9" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="5">
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="4">
         <v>45231</v>
       </c>
       <c r="F13" s="6">
         <v>0.10416666666666667</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>45231</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="5">
         <v>0.21875</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:9" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>45233</v>
       </c>
       <c r="F14" s="6">
         <v>0.46875</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>45233</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="5">
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:9" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>45235</v>
       </c>
       <c r="F15" s="6">
         <v>0.85416666666666663</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>45236</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="5">
         <v>0.17708333333333334</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:9" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>45238</v>
       </c>
       <c r="F16" s="6">
         <v>0.32291666666666669</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>45238</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="5">
         <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="5">
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4">
         <v>45240</v>
       </c>
       <c r="F17" s="6">
         <v>0.54166666666666663</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <v>45240</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="5">
         <v>0.65625</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="5">
+      <c r="D18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="4">
         <v>45242</v>
       </c>
       <c r="F18" s="6">
         <v>0.47916666666666669</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>45242</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="5">
         <v>0.61458333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>45245</v>
       </c>
       <c r="F19" s="6">
         <v>0.34375</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <v>45245</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="5">
         <v>0.53125</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="5">
+      <c r="D20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4">
         <v>45247</v>
       </c>
       <c r="F20" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>45247</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="5">
         <v>0.71875</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="5">
+      <c r="D21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="4">
         <v>45250</v>
       </c>
       <c r="F21" s="6">
         <v>0.65625</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <v>45250</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="5">
         <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>45252</v>
       </c>
       <c r="F22" s="6">
         <v>0.39583333333333331</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>45252</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="5">
         <v>0.48958333333333331</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>45255</v>
       </c>
       <c r="F23" s="6">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
         <v>45255</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="5">
         <v>0.5625</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="5">
+      <c r="D24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="4">
         <v>45258</v>
       </c>
       <c r="F24" s="6">
         <v>0.94791666666666663</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="4">
         <v>45259</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="5">
         <v>0.13541666666666666</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>45262</v>
       </c>
       <c r="F25" s="6">
         <v>0.35416666666666669</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <v>45262</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="5">
         <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="5">
+      <c r="D26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="4">
         <v>45265</v>
       </c>
       <c r="F26" s="6">
         <v>0.57291666666666663</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>45265</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="5">
         <v>0.6875</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="4">
         <v>45268</v>
       </c>
       <c r="F27" s="6">
         <v>0.63541666666666663</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
         <v>45268</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="5">
         <v>0.82291666666666663</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="5">
+      <c r="D28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="4">
         <v>45271</v>
       </c>
       <c r="F28" s="6">
         <v>0.375</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <v>45271</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="5">
         <v>0.5625</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="4">
         <v>45274</v>
       </c>
       <c r="F29" s="6">
         <v>0.48958333333333331</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="4">
         <v>45274</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="5">
         <v>0.625</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="4">
         <v>45277</v>
       </c>
       <c r="F30" s="6">
         <v>0.79166666666666663</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="4">
         <v>45277</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="5">
         <v>0.96875</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="5">
+      <c r="D31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="4">
         <v>45280</v>
       </c>
       <c r="F31" s="6">
         <v>0.5</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="4">
         <v>45280</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="5">
         <v>0.64583333333333337</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="4">
         <v>45283</v>
       </c>
       <c r="F32" s="6">
         <v>0.4375</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="4">
         <v>45283</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="5">
         <v>0.61458333333333337</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="4">
         <v>45286</v>
       </c>
       <c r="F33" s="6">
         <v>0.63541666666666663</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="4">
         <v>45286</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="5">
         <v>0.77083333333333337</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="4">
         <v>45289</v>
       </c>
       <c r="F34" s="6">
         <v>0.98958333333333337</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="4">
         <v>45290</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="5">
         <v>0.13541666666666666</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="5">
+      <c r="D35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="4">
         <v>45293</v>
       </c>
       <c r="F35" s="6">
         <v>0.5625</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="4">
         <v>45293</v>
       </c>
-      <c r="H35" s="7">
+      <c r="H35" s="5">
         <v>0.73958333333333337</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="4">
         <v>45296</v>
       </c>
       <c r="F36" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="4">
         <v>45296</v>
       </c>
-      <c r="H36" s="7">
+      <c r="H36" s="5">
         <v>0.77083333333333337</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="5">
+      <c r="D37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="4">
         <v>45299</v>
       </c>
       <c r="F37" s="6">
         <v>0.39583333333333331</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="4">
         <v>45299</v>
       </c>
-      <c r="H37" s="7">
+      <c r="H37" s="5">
         <v>0.48958333333333331</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="4">
         <v>45302</v>
       </c>
       <c r="F38" s="6">
         <v>0.42708333333333331</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="4">
         <v>45302</v>
       </c>
-      <c r="H38" s="7">
+      <c r="H38" s="5">
         <v>0.57291666666666663</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="4">
         <v>45305</v>
       </c>
       <c r="F39" s="6">
         <v>0.47916666666666669</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="4">
         <v>45305</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="5">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="5">
+      <c r="D40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="4">
         <v>45308</v>
       </c>
       <c r="F40" s="6">
         <v>0.125</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="4">
         <v>45308</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="5">
         <v>0.26041666666666669</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="4">
         <v>45311</v>
       </c>
       <c r="F41" s="6">
         <v>0.32291666666666669</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="4">
         <v>45311</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="5">
         <v>0.46875</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="5">
+      <c r="D42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="4">
         <v>45314</v>
       </c>
       <c r="F42" s="6">
         <v>0.5625</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="4">
         <v>45314</v>
       </c>
-      <c r="H42" s="7">
+      <c r="H42" s="5">
         <v>0.73958333333333337</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="4">
         <v>45317</v>
       </c>
       <c r="F43" s="6">
         <v>0.84375</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="4">
         <v>45318</v>
       </c>
-      <c r="H43" s="7">
+      <c r="H43" s="5">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="5">
+      <c r="D44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="4">
         <v>45320</v>
       </c>
       <c r="F44" s="6">
         <v>0.65625</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G44" s="4">
         <v>45320</v>
       </c>
-      <c r="H44" s="7">
+      <c r="H44" s="5">
         <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="4">
         <v>45323</v>
       </c>
       <c r="F45" s="6">
         <v>0.25</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45" s="4">
         <v>45323</v>
       </c>
-      <c r="H45" s="7">
+      <c r="H45" s="5">
         <v>0.38541666666666669</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="5">
+      <c r="D46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="4">
         <v>45326</v>
       </c>
       <c r="F46" s="6">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46" s="4">
         <v>45326</v>
       </c>
-      <c r="H46" s="7">
+      <c r="H46" s="5">
         <v>0.65625</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="4" t="s">
+      <c r="C47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="4">
         <v>45329</v>
       </c>
       <c r="F47" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G47" s="4">
         <v>45329</v>
       </c>
-      <c r="H47" s="7">
+      <c r="H47" s="5">
         <v>0.46875</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="5">
+      <c r="D48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="4">
         <v>45332</v>
       </c>
       <c r="F48" s="6">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48" s="4">
         <v>45332</v>
       </c>
-      <c r="H48" s="7">
+      <c r="H48" s="5">
         <v>0.65625</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="4">
         <v>45335</v>
       </c>
       <c r="F49" s="6">
         <v>0.61458333333333337</v>
       </c>
-      <c r="G49" s="5">
+      <c r="G49" s="4">
         <v>45335</v>
       </c>
-      <c r="H49" s="7">
+      <c r="H49" s="5">
         <v>0.75</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="4">
         <v>45338</v>
       </c>
       <c r="F50" s="6">
         <v>0.13541666666666666</v>
       </c>
-      <c r="G50" s="5">
+      <c r="G50" s="4">
         <v>45338</v>
       </c>
-      <c r="H50" s="7">
+      <c r="H50" s="5">
         <v>0.3125</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="5">
+      <c r="D51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="4">
         <v>45341</v>
       </c>
       <c r="F51" s="6">
         <v>0.70833333333333337</v>
       </c>
-      <c r="G51" s="5">
+      <c r="G51" s="4">
         <v>45341</v>
       </c>
-      <c r="H51" s="7">
+      <c r="H51" s="5">
         <v>0.84375</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="4">
         <v>45344</v>
       </c>
       <c r="F52" s="6">
         <v>0.27083333333333331</v>
       </c>
-      <c r="G52" s="5">
+      <c r="G52" s="4">
         <v>45344</v>
       </c>
-      <c r="H52" s="7">
+      <c r="H52" s="5">
         <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" s="5">
+      <c r="D53" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="4">
         <v>45347</v>
       </c>
       <c r="F53" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G53" s="5">
+      <c r="G53" s="4">
         <v>45347</v>
       </c>
-      <c r="H53" s="7">
+      <c r="H53" s="5">
         <v>0.46875</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54" s="4">
         <v>45350</v>
       </c>
       <c r="F54" s="6">
         <v>0.88541666666666663</v>
       </c>
-      <c r="G54" s="5">
+      <c r="G54" s="4">
         <v>45351</v>
       </c>
-      <c r="H54" s="7">
+      <c r="H54" s="5">
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="5">
+      <c r="D55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="4">
         <v>45354</v>
       </c>
       <c r="F55" s="6">
         <v>0.48958333333333331</v>
       </c>
-      <c r="G55" s="5">
+      <c r="G55" s="4">
         <v>45354</v>
       </c>
-      <c r="H55" s="7">
+      <c r="H55" s="5">
         <v>0.625</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="72" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E56" s="5">
+      <c r="E56" s="4">
         <v>45357</v>
       </c>
       <c r="F56" s="6">
         <v>0.5625</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G56" s="4">
         <v>45357</v>
       </c>
-      <c r="H56" s="7">
+      <c r="H56" s="5">
         <v>0.65625</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57" s="4">
         <v>45360</v>
       </c>
       <c r="F57" s="6">
         <v>0.65625</v>
       </c>
-      <c r="G57" s="5">
+      <c r="G57" s="4">
         <v>45360</v>
       </c>
-      <c r="H57" s="7">
+      <c r="H57" s="5">
         <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E58" s="5">
+      <c r="D58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="4">
         <v>45363</v>
       </c>
       <c r="F58" s="6">
         <v>0.1875</v>
       </c>
-      <c r="G58" s="5">
+      <c r="G58" s="4">
         <v>45363</v>
       </c>
-      <c r="H58" s="7">
+      <c r="H58" s="5">
         <v>0.375</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E59" s="5">
+      <c r="E59" s="4">
         <v>45366</v>
       </c>
       <c r="F59" s="6">
         <v>0.77083333333333337</v>
       </c>
-      <c r="G59" s="5">
+      <c r="G59" s="4">
         <v>45366</v>
       </c>
-      <c r="H59" s="7">
+      <c r="H59" s="5">
         <v>0.90625</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" s="4" t="s">
+      <c r="C60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E60" s="5">
+      <c r="E60" s="4">
         <v>45369</v>
       </c>
       <c r="F60" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="G60" s="5">
+      <c r="G60" s="4">
         <v>45369</v>
       </c>
-      <c r="H60" s="7">
+      <c r="H60" s="5">
         <v>0.59375</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="86.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D61" s="4" t="s">
+      <c r="C61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E61" s="5">
+      <c r="E61" s="4">
         <v>45372</v>
       </c>
       <c r="F61" s="6">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G61" s="5">
+      <c r="G61" s="4">
         <v>45372</v>
       </c>
-      <c r="H61" s="7">
+      <c r="H61" s="5">
         <v>0.63541666666666663</v>
       </c>
     </row>

</xml_diff>